<commit_message>
Create Screenshots and Readme
</commit_message>
<xml_diff>
--- a/here.xlsx
+++ b/here.xlsx
@@ -7,94 +7,10 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Page 1 - Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Meaning</t>
-  </si>
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Probably extinct</t>
-  </si>
-  <si>
-    <t>Taxa and populations that inhabited Russian territory or marine
-areain the past and whose presence has been unconfirmed for
-the last 50years</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Endangered</t>
-  </si>
-  <si>
-    <t>Taxa and populations whose abundance has decreased to critical
-levels,allowing them to become extinct in the near future</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Decreasing number</t>
-  </si>
-  <si>
-    <t>Taxa and populations whose number is constantly decreasing.If
-the negative factors reducing the populations continue,the taxa
-can be moved to Category 1 in the near future.</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Rare</t>
-  </si>
-  <si>
-    <t>Taxa and populations with a low number of individuals inhabiting
-limited territory or marine area  or sporadically distributed over
-extensive terntory or marine area</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Uncertain status</t>
-  </si>
-  <si>
-    <t>Taxa and populations which apparently belong to one of the
-above categories but there are considerable gaps in knowledge of
-them or they do not exactly meet the criteria for the othet
-categories.</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Renabiitated and renabilitating</t>
-  </si>
-  <si>
-    <t>Taxa and populations whose number and distribution is recovered
-or recovering due to protective measures.They are close to the
-state of stable existence without any current urgent measures on
-protection and rehabilitation</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -116,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -124,30 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,106 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C2"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>